<commit_message>
Arreglo de Modelado de Dominio
</commit_message>
<xml_diff>
--- a/MuestreoDatosSpaOnline.xlsx
+++ b/MuestreoDatosSpaOnline.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://grchia-my.sharepoint.com/personal/jhonatan_gomez_wiga_io/Documents/Escritorio/UCO/DOO GIT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="619" documentId="8_{27DC0606-9BCB-400A-8EF6-FE9749DE6261}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AAB97841-70B4-4FCD-81A9-5D95218D763F}"/>
+  <xr:revisionPtr revIDLastSave="620" documentId="8_{27DC0606-9BCB-400A-8EF6-FE9749DE6261}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9FA8676B-963B-431D-A08E-03D48734B2E8}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="5" activeTab="11" xr2:uid="{977484E6-24A6-47C7-9A52-E0B99E486A9A}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="69">
   <si>
     <t>Identificador</t>
   </si>
@@ -110,9 +110,6 @@
   </si>
   <si>
     <t>Fecha inicio</t>
-  </si>
-  <si>
-    <t>Fecha Fin</t>
   </si>
   <si>
     <t>CitaReserva</t>
@@ -264,7 +261,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -470,7 +467,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -482,7 +479,6 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="2" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -507,10 +503,10 @@
     <xf numFmtId="14" fontId="0" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="12" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="16" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="16" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="17" borderId="1" xfId="2" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="16" borderId="1" xfId="2" applyFill="1" applyBorder="1"/>
@@ -864,7 +860,7 @@
   <dimension ref="B2:G16"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -890,14 +886,14 @@
       </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B3" s="12">
+      <c r="B3" s="11">
         <v>1</v>
       </c>
-      <c r="C3" s="13" t="str">
+      <c r="C3" s="12" t="str">
         <f>TipoServicio!D4</f>
         <v>Facial</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="11" t="s">
         <v>2</v>
       </c>
       <c r="E3" s="3" t="str">
@@ -906,14 +902,14 @@
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B4" s="14">
+      <c r="B4" s="13">
         <v>2</v>
       </c>
-      <c r="C4" s="15" t="str">
+      <c r="C4" s="14" t="str">
         <f>TipoServicio!D4</f>
         <v>Facial</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="D4" s="13" t="s">
         <v>3</v>
       </c>
       <c r="E4" s="3" t="str">
@@ -925,7 +921,7 @@
       <c r="B5" s="4">
         <v>3</v>
       </c>
-      <c r="C5" s="16" t="str">
+      <c r="C5" s="15" t="str">
         <f>TipoServicio!D4</f>
         <v>Facial</v>
       </c>
@@ -938,14 +934,14 @@
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B6" s="17">
+      <c r="B6" s="16">
         <v>4</v>
       </c>
-      <c r="C6" s="18" t="str">
+      <c r="C6" s="17" t="str">
         <f>TipoServicio!D4</f>
         <v>Facial</v>
       </c>
-      <c r="D6" s="17" t="s">
+      <c r="D6" s="16" t="s">
         <v>6</v>
       </c>
       <c r="E6" s="3" t="str">
@@ -954,13 +950,13 @@
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B7" s="19">
+      <c r="B7" s="18">
         <v>5</v>
       </c>
-      <c r="C7" s="20" t="s">
+      <c r="C7" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="19" t="s">
+      <c r="D7" s="18" t="s">
         <v>5</v>
       </c>
       <c r="E7" s="3" t="str">
@@ -969,13 +965,13 @@
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B8" s="21">
+      <c r="B8" s="20">
         <v>6</v>
       </c>
-      <c r="C8" s="22" t="s">
+      <c r="C8" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="21" t="s">
+      <c r="D8" s="20" t="s">
         <v>7</v>
       </c>
       <c r="E8" s="3" t="str">
@@ -987,7 +983,7 @@
       <c r="B9" s="5">
         <v>7</v>
       </c>
-      <c r="C9" s="23" t="str">
+      <c r="C9" s="22" t="str">
         <f>TipoServicio!D9</f>
         <v>Corporal</v>
       </c>
@@ -1000,14 +996,14 @@
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B10" s="24">
+      <c r="B10" s="23">
         <v>8</v>
       </c>
-      <c r="C10" s="25" t="str">
+      <c r="C10" s="24" t="str">
         <f>TipoServicio!D5</f>
         <v>Manicura</v>
       </c>
-      <c r="D10" s="24" t="s">
+      <c r="D10" s="23" t="s">
         <v>18</v>
       </c>
       <c r="E10" s="3" t="str">
@@ -1052,10 +1048,10 @@
         <v>0</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>13</v>
@@ -1065,12 +1061,12 @@
       <c r="B4" s="7">
         <v>1</v>
       </c>
-      <c r="C4" s="45" t="str">
+      <c r="C4" s="44" t="str">
         <f>CitaReserva!I3</f>
         <v>1-11/01/2024  8-Facial-Limpieza Facial Profunda</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E4" s="3" t="str">
         <f>C4&amp;"-"&amp;D4</f>
@@ -1081,12 +1077,12 @@
       <c r="B5" s="5">
         <v>2</v>
       </c>
-      <c r="C5" s="23" t="str">
+      <c r="C5" s="22" t="str">
         <f>CitaReserva!I4</f>
         <v>2-15/02/2024 10-Facial-Limpieza facial premium</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E5" s="3" t="str">
         <f t="shared" ref="E5:E6" si="0">C5&amp;"-"&amp;D5</f>
@@ -1094,15 +1090,15 @@
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="46">
+      <c r="B6" s="45">
         <v>3</v>
       </c>
-      <c r="C6" s="47" t="str">
+      <c r="C6" s="46" t="str">
         <f>CitaReservaServicio!E6</f>
         <v>3-Manicura-Manicura Pies y Manos</v>
       </c>
-      <c r="D6" s="46" t="s">
-        <v>54</v>
+      <c r="D6" s="45" t="s">
+        <v>53</v>
       </c>
       <c r="E6" s="3" t="str">
         <f t="shared" si="0"/>
@@ -1140,29 +1136,29 @@
         <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>57</v>
-      </c>
       <c r="E2" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B3" s="12">
+      <c r="B3" s="11">
         <v>1</v>
       </c>
-      <c r="C3" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="E3" s="13" t="str">
+      <c r="C3" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="E3" s="12" t="str">
         <f>Inventario!E4</f>
         <v>Inventario1</v>
       </c>
@@ -1172,16 +1168,16 @@
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="17">
+      <c r="B4" s="16">
         <v>2</v>
       </c>
-      <c r="C4" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="D4" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="E4" s="18" t="str">
+      <c r="C4" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="E4" s="17" t="str">
         <f>Inventario!E5</f>
         <v>Inventario2</v>
       </c>
@@ -1191,16 +1187,16 @@
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="49">
+      <c r="B5" s="48">
         <v>3</v>
       </c>
-      <c r="C5" s="49" t="s">
-        <v>60</v>
-      </c>
-      <c r="D5" s="49" t="s">
-        <v>62</v>
-      </c>
-      <c r="E5" s="50" t="str">
+      <c r="C5" s="48" t="s">
+        <v>59</v>
+      </c>
+      <c r="D5" s="48" t="s">
+        <v>61</v>
+      </c>
+      <c r="E5" s="49" t="str">
         <f>Inventario!E6</f>
         <v>Inventario3</v>
       </c>
@@ -1224,7 +1220,7 @@
   <dimension ref="B3:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1238,23 +1234,23 @@
         <v>0</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="17">
+      <c r="B4" s="16">
         <v>1</v>
       </c>
-      <c r="C4" s="17" t="s">
-        <v>65</v>
-      </c>
-      <c r="D4" s="18" t="str">
+      <c r="C4" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="D4" s="17" t="str">
         <f>Sucursal!F3</f>
         <v>Spa Marinilla</v>
       </c>
@@ -1264,13 +1260,13 @@
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="46">
+      <c r="B5" s="45">
         <v>2</v>
       </c>
-      <c r="C5" s="46" t="s">
-        <v>66</v>
-      </c>
-      <c r="D5" s="47" t="str">
+      <c r="C5" s="45" t="s">
+        <v>65</v>
+      </c>
+      <c r="D5" s="46" t="str">
         <f>Sucursal!F4</f>
         <v>Spa Rionegro</v>
       </c>
@@ -1280,13 +1276,13 @@
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="12">
+      <c r="B6" s="11">
         <v>3</v>
       </c>
-      <c r="C6" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="D6" s="13" t="str">
+      <c r="C6" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="D6" s="12" t="str">
         <f>Sucursal!F5</f>
         <v>Spa Medellin</v>
       </c>
@@ -1307,7 +1303,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C21B0B2-4AE8-428E-B02F-213E8BCC7E65}">
-  <dimension ref="B3:G11"/>
+  <dimension ref="B3:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A15" sqref="A10:A15"/>
@@ -1319,7 +1315,7 @@
     <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -1330,7 +1326,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" s="4">
         <v>1</v>
       </c>
@@ -1341,9 +1337,8 @@
         <f>C4</f>
         <v>Facial</v>
       </c>
-      <c r="G4" s="11"/>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" s="5">
         <v>2</v>
       </c>
@@ -1355,7 +1350,7 @@
         <v>Manicura</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="6">
         <v>3</v>
       </c>
@@ -1367,7 +1362,7 @@
         <v>Pedicura</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" s="7">
         <v>4</v>
       </c>
@@ -1379,7 +1374,7 @@
         <v>Depilacion</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B8" s="8">
         <v>5</v>
       </c>
@@ -1391,7 +1386,7 @@
         <v>Sauna</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B9" s="9">
         <v>6</v>
       </c>
@@ -1402,9 +1397,6 @@
         <f t="shared" si="0"/>
         <v>Corporal</v>
       </c>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D11" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1414,20 +1406,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED7F291D-B295-40DB-B7D1-5B0FE6D38210}">
-  <dimension ref="B2:J17"/>
+  <dimension ref="B2:I17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="30" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="40.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="40.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1441,125 +1433,109 @@
         <v>20</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="H2" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B3" s="26">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B3" s="25">
         <v>1</v>
       </c>
-      <c r="C3" s="27" t="str">
+      <c r="C3" s="26" t="str">
         <f>Servicio!E3</f>
         <v>Facial-Limpieza Facial Profunda</v>
       </c>
-      <c r="D3" s="28">
+      <c r="D3" s="27">
         <v>0.01</v>
       </c>
-      <c r="E3" s="29">
+      <c r="E3" s="28">
         <v>45292</v>
       </c>
-      <c r="F3" s="29">
-        <v>45324</v>
-      </c>
-      <c r="G3" s="52" t="str">
+      <c r="F3" s="51" t="str">
         <f>Notificacion!D3</f>
         <v>True</v>
       </c>
-      <c r="H3" s="3" t="str">
+      <c r="G3" s="3" t="str">
         <f>C3&amp;"--"&amp;D3</f>
         <v>Facial-Limpieza Facial Profunda--0,01</v>
       </c>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" s="5">
         <v>2</v>
       </c>
-      <c r="C4" s="23" t="str">
+      <c r="C4" s="22" t="str">
         <f>Servicio!E5</f>
         <v>Facial-Limpieza facial premium</v>
       </c>
-      <c r="D4" s="30">
+      <c r="D4" s="29">
         <v>0.04</v>
       </c>
-      <c r="E4" s="31">
+      <c r="E4" s="30">
         <v>45293</v>
       </c>
-      <c r="F4" s="31">
-        <v>45325</v>
-      </c>
-      <c r="G4" s="5" t="str">
+      <c r="F4" s="5" t="str">
         <f>Notificacion!D4</f>
         <v>False</v>
       </c>
-      <c r="H4" s="3" t="str">
-        <f t="shared" ref="H4:H6" si="0">C4&amp;"--"&amp;D4</f>
+      <c r="G4" s="3" t="str">
+        <f t="shared" ref="G4:G6" si="0">C4&amp;"--"&amp;D4</f>
         <v>Facial-Limpieza facial premium--0,04</v>
       </c>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B5" s="17">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B5" s="16">
         <v>3</v>
       </c>
-      <c r="C5" s="18" t="str">
+      <c r="C5" s="17" t="str">
         <f>Servicio!E8</f>
         <v>Facial-dermaplaning + alta hidratación</v>
       </c>
-      <c r="D5" s="32">
+      <c r="D5" s="31">
         <v>0.12</v>
       </c>
-      <c r="E5" s="33">
+      <c r="E5" s="32">
         <v>45294</v>
       </c>
-      <c r="F5" s="33">
-        <v>45326</v>
-      </c>
-      <c r="G5" s="17" t="str">
+      <c r="F5" s="16" t="str">
         <f>Notificacion!D4</f>
         <v>False</v>
       </c>
-      <c r="H5" s="3" t="str">
+      <c r="G5" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Facial-dermaplaning + alta hidratación--0,12</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B6" s="19">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B6" s="18">
         <v>4</v>
       </c>
-      <c r="C6" s="20" t="str">
+      <c r="C6" s="19" t="str">
         <f>Servicio!E9</f>
         <v>Corporal-Masaje Relajante Premium</v>
       </c>
-      <c r="D6" s="34">
+      <c r="D6" s="33">
         <v>0.15</v>
       </c>
-      <c r="E6" s="35">
+      <c r="E6" s="34">
         <v>45295</v>
       </c>
-      <c r="F6" s="35">
-        <v>45327</v>
-      </c>
-      <c r="G6" s="19" t="str">
+      <c r="F6" s="18" t="str">
         <f>Notificacion!D3</f>
         <v>True</v>
       </c>
-      <c r="H6" s="3" t="str">
+      <c r="G6" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Corporal-Masaje Relajante Premium--0,15</v>
       </c>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="J9" s="10"/>
-    </row>
-    <row r="17" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I9" s="10"/>
+    </row>
+    <row r="17" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F17" s="10"/>
-      <c r="G17" s="10"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1567,7 +1543,7 @@
     <hyperlink ref="C4" location="Servicio!E5" display="Servicio!E5" xr:uid="{055A6C60-BCE9-4620-92D7-17BD302ABA53}"/>
     <hyperlink ref="C5" location="Ofertas!E8" display="Ofertas!E8" xr:uid="{1B6DC2A7-68E4-415B-8C1B-D99BC18AF5B8}"/>
     <hyperlink ref="C6" location="Ofertas!E9" display="Ofertas!E9" xr:uid="{9FCC7121-5D91-481B-91AC-D0370760E88E}"/>
-    <hyperlink ref="G3" location="Notificacion!D3" display="Notificacion!D3" xr:uid="{1BB13AF6-17C5-45FB-BBEB-D22C765F3DB1}"/>
+    <hyperlink ref="F3" location="Notificacion!D3" display="Notificacion!D3" xr:uid="{1BB13AF6-17C5-45FB-BBEB-D22C765F3DB1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1591,18 +1567,18 @@
         <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B3" s="51">
+      <c r="B3" s="50">
         <v>1</v>
       </c>
-      <c r="C3" s="51" t="s">
-        <v>54</v>
+      <c r="C3" s="50" t="s">
+        <v>53</v>
       </c>
       <c r="D3" s="3" t="str">
         <f>C3</f>
@@ -1610,11 +1586,11 @@
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B4" s="48">
+      <c r="B4" s="47">
         <v>2</v>
       </c>
-      <c r="C4" s="48" t="s">
-        <v>55</v>
+      <c r="C4" s="47" t="s">
+        <v>54</v>
       </c>
       <c r="D4" s="3" t="str">
         <f>C4</f>
@@ -1649,7 +1625,7 @@
         <v>14</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>13</v>
@@ -1659,11 +1635,11 @@
       <c r="B4" s="4">
         <v>1</v>
       </c>
-      <c r="C4" s="16" t="str">
+      <c r="C4" s="15" t="str">
         <f>Servicio!E3</f>
         <v>Facial-Limpieza Facial Profunda</v>
       </c>
-      <c r="D4" s="16">
+      <c r="D4" s="15">
         <f>CitaReserva!B3</f>
         <v>1</v>
       </c>
@@ -1676,11 +1652,11 @@
       <c r="B5" s="5">
         <v>2</v>
       </c>
-      <c r="C5" s="23" t="str">
+      <c r="C5" s="22" t="str">
         <f>Servicio!E6</f>
         <v>Facial-Limpieza facial + hydrodermoabrasión</v>
       </c>
-      <c r="D5" s="23">
+      <c r="D5" s="22">
         <f>CitaReserva!B4</f>
         <v>2</v>
       </c>
@@ -1690,14 +1666,14 @@
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="19">
+      <c r="B6" s="18">
         <v>3</v>
       </c>
-      <c r="C6" s="20" t="str">
+      <c r="C6" s="19" t="str">
         <f>Servicio!E10</f>
         <v>Manicura-Manicura Pies y Manos</v>
       </c>
-      <c r="D6" s="20">
+      <c r="D6" s="19">
         <f>CitaReserva!B5</f>
         <v>3</v>
       </c>
@@ -1722,7 +1698,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{945BD593-8DF0-43F2-BE97-815884B39FA6}">
   <dimension ref="B2:I5"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
@@ -1743,22 +1719,22 @@
         <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>13</v>
@@ -1768,26 +1744,26 @@
       <c r="B3" s="4">
         <v>1</v>
       </c>
-      <c r="C3" s="36" t="s">
-        <v>28</v>
+      <c r="C3" s="35" t="s">
+        <v>27</v>
       </c>
       <c r="D3" s="4" t="str">
         <f>Servicio!E3</f>
         <v>Facial-Limpieza Facial Profunda</v>
       </c>
-      <c r="E3" s="16" t="str">
+      <c r="E3" s="15" t="str">
         <f>Consentimiento!E4</f>
         <v>1-11/01/2024  8-Facial-Limpieza Facial Profunda-True</v>
       </c>
-      <c r="F3" s="16" t="str">
+      <c r="F3" s="15" t="str">
         <f>Sucursal!F3</f>
         <v>Spa Marinilla</v>
       </c>
-      <c r="G3" s="16" t="str">
+      <c r="G3" s="15" t="str">
         <f>Usuario!C4</f>
         <v>jhonatan12353@gmail.com</v>
       </c>
-      <c r="H3" s="16" t="str">
+      <c r="H3" s="15" t="str">
         <f>Pago!E4</f>
         <v>Bancolombia-True</v>
       </c>
@@ -1797,29 +1773,29 @@
       </c>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B4" s="37">
+      <c r="B4" s="36">
         <v>2</v>
       </c>
-      <c r="C4" s="38" t="s">
-        <v>29</v>
-      </c>
-      <c r="D4" s="37" t="str">
+      <c r="C4" s="37" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="36" t="str">
         <f>Servicio!E5</f>
         <v>Facial-Limpieza facial premium</v>
       </c>
-      <c r="E4" s="42" t="str">
+      <c r="E4" s="41" t="str">
         <f>Consentimiento!E5</f>
         <v>2-15/02/2024 10-Facial-Limpieza facial premium-False</v>
       </c>
-      <c r="F4" s="42" t="str">
+      <c r="F4" s="41" t="str">
         <f>Sucursal!F4</f>
         <v>Spa Rionegro</v>
       </c>
-      <c r="G4" s="42" t="str">
+      <c r="G4" s="41" t="str">
         <f>Usuario!C5</f>
         <v>jhonatan12353@hotmail.com</v>
       </c>
-      <c r="H4" s="42" t="str">
+      <c r="H4" s="41" t="str">
         <f>Pago!E7</f>
         <v>Banco de Occidente-True</v>
       </c>
@@ -1832,26 +1808,26 @@
       <c r="B5" s="6">
         <v>3</v>
       </c>
-      <c r="C5" s="39" t="s">
-        <v>30</v>
+      <c r="C5" s="38" t="s">
+        <v>29</v>
       </c>
       <c r="D5" s="6" t="str">
         <f>Servicio!E10</f>
         <v>Manicura-Manicura Pies y Manos</v>
       </c>
-      <c r="E5" s="43" t="str">
+      <c r="E5" s="42" t="str">
         <f>Consentimiento!E6</f>
         <v>3-Manicura-Manicura Pies y Manos-True</v>
       </c>
-      <c r="F5" s="43" t="str">
+      <c r="F5" s="42" t="str">
         <f>Sucursal!F5</f>
         <v>Spa Medellin</v>
       </c>
-      <c r="G5" s="43" t="str">
+      <c r="G5" s="42" t="str">
         <f>Usuario!C6</f>
         <v>jhonatan.gomez9180@uco.net.co</v>
       </c>
-      <c r="H5" s="43" t="str">
+      <c r="H5" s="42" t="str">
         <f>Pago!E8</f>
         <v>Banco Itaú-False</v>
       </c>
@@ -1884,7 +1860,7 @@
   <dimension ref="B3:I17"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B6"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1901,47 +1877,47 @@
         <v>0</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>34</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B4" s="40">
+      <c r="B4" s="39">
         <v>1</v>
       </c>
-      <c r="C4" s="41" t="s">
-        <v>45</v>
-      </c>
-      <c r="D4" s="40" t="s">
+      <c r="C4" s="40" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4" s="39" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4" s="39" t="s">
         <v>38</v>
       </c>
-      <c r="E4" s="40" t="s">
-        <v>39</v>
-      </c>
-      <c r="F4" s="40">
+      <c r="F4" s="39">
         <v>1038419180</v>
       </c>
-      <c r="G4" s="40">
+      <c r="G4" s="39">
         <v>3246828223</v>
       </c>
-      <c r="H4" s="41" t="str">
+      <c r="H4" s="40" t="str">
         <f>TipoUsuario!D4</f>
         <v>Administrador</v>
       </c>
@@ -1951,25 +1927,25 @@
       </c>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B5" s="24">
+      <c r="B5" s="23">
         <v>2</v>
       </c>
-      <c r="C5" s="25" t="s">
-        <v>36</v>
-      </c>
-      <c r="D5" s="24" t="s">
+      <c r="C5" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="E5" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="E5" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="F5" s="24">
+      <c r="F5" s="23">
         <v>1038419181</v>
       </c>
-      <c r="G5" s="24">
+      <c r="G5" s="23">
         <v>3246828223</v>
       </c>
-      <c r="H5" s="25" t="str">
+      <c r="H5" s="24" t="str">
         <f>TipoUsuario!D5</f>
         <v>Empleado</v>
       </c>
@@ -1982,14 +1958,14 @@
       <c r="B6" s="4">
         <v>3</v>
       </c>
-      <c r="C6" s="16" t="s">
+      <c r="C6" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="E6" s="4" t="s">
         <v>38</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>39</v>
       </c>
       <c r="F6" s="4">
         <v>1038419182</v>
@@ -1997,7 +1973,7 @@
       <c r="G6" s="4">
         <v>3246828223</v>
       </c>
-      <c r="H6" s="16" t="str">
+      <c r="H6" s="15" t="str">
         <f>TipoUsuario!D6</f>
         <v>Cliente</v>
       </c>
@@ -2041,7 +2017,7 @@
         <v>0</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>13</v>
@@ -2052,7 +2028,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D4" s="3" t="str">
         <f>C4</f>
@@ -2060,11 +2036,11 @@
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B5" s="19">
+      <c r="B5" s="18">
         <v>2</v>
       </c>
-      <c r="C5" s="19" t="s">
-        <v>42</v>
+      <c r="C5" s="18" t="s">
+        <v>41</v>
       </c>
       <c r="D5" s="3" t="str">
         <f t="shared" ref="D5:D6" si="0">C5</f>
@@ -2076,7 +2052,7 @@
         <v>3</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D6" s="3" t="str">
         <f t="shared" si="0"/>
@@ -2093,7 +2069,7 @@
   <dimension ref="B3:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2108,23 +2084,23 @@
         <v>0</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="26">
+      <c r="B4" s="25">
         <v>1</v>
       </c>
-      <c r="C4" s="26" t="s">
-        <v>47</v>
-      </c>
-      <c r="D4" s="27" t="str">
+      <c r="C4" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="D4" s="26" t="str">
         <f>Notificacion!D3</f>
         <v>True</v>
       </c>
@@ -2138,9 +2114,9 @@
         <v>2</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="D5" s="23" t="str">
+        <v>47</v>
+      </c>
+      <c r="D5" s="22" t="str">
         <f>Notificacion!D4</f>
         <v>False</v>
       </c>
@@ -2155,9 +2131,9 @@
         <v>3</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="D6" s="43" t="str">
+        <v>48</v>
+      </c>
+      <c r="D6" s="42" t="str">
         <f>Notificacion!D3</f>
         <v>True</v>
       </c>
@@ -2171,9 +2147,9 @@
         <v>4</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="D7" s="45" t="str">
+        <v>49</v>
+      </c>
+      <c r="D7" s="44" t="str">
         <f>Notificacion!D3</f>
         <v>True</v>
       </c>
@@ -2183,13 +2159,13 @@
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="44">
+      <c r="B8" s="43">
         <v>5</v>
       </c>
-      <c r="C8" s="44" t="s">
-        <v>51</v>
-      </c>
-      <c r="D8" s="53" t="str">
+      <c r="C8" s="43" t="s">
+        <v>50</v>
+      </c>
+      <c r="D8" s="52" t="str">
         <f>Notificacion!D4</f>
         <v>False</v>
       </c>

</xml_diff>

<commit_message>
Ajuste diseños muesteo de datos
</commit_message>
<xml_diff>
--- a/MuestreoDatosSpaOnline.xlsx
+++ b/MuestreoDatosSpaOnline.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://grchia-my.sharepoint.com/personal/jhonatan_gomez_wiga_io/Documents/Escritorio/UCO/DOO GIT/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DOO\DOO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="856" documentId="8_{27DC0606-9BCB-400A-8EF6-FE9749DE6261}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{174844B4-90D5-41FA-B8EE-0B2777A1CF2F}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9BD2F17-69E2-4242-9FD8-7288A58A037D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-4815" windowWidth="29040" windowHeight="15720" firstSheet="9" activeTab="14" xr2:uid="{977484E6-24A6-47C7-9A52-E0B99E486A9A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="1" activeTab="18" xr2:uid="{977484E6-24A6-47C7-9A52-E0B99E486A9A}"/>
   </bookViews>
   <sheets>
     <sheet name="SpaOnline" sheetId="16" r:id="rId1"/>
@@ -322,9 +322,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-    <numFmt numFmtId="168" formatCode="_-[$$-240A]\ * #,##0.00_-;\-[$$-240A]\ * #,##0.00_-;_-[$$-240A]\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="166" formatCode="_-[$$-240A]\ * #,##0.00_-;\-[$$-240A]\ * #,##0.00_-;_-[$$-240A]\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -542,7 +542,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -580,10 +580,10 @@
     <xf numFmtId="14" fontId="0" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="12" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="16" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="16" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="17" borderId="1" xfId="2" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="16" borderId="1" xfId="2" applyFill="1" applyBorder="1"/>
@@ -598,14 +598,14 @@
     <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="3" fillId="15" borderId="1" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="18" borderId="1" xfId="2" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="3" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="11" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="12" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="13" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="4" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="14" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="11" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="12" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="13" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="4" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="14" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="22" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="19" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
@@ -948,7 +948,7 @@
   <dimension ref="B3:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="B1" sqref="B1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -998,11 +998,13 @@
   <dimension ref="B3:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="B1" sqref="B1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1039,11 +1041,13 @@
   <dimension ref="B3:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1080,11 +1084,12 @@
   <dimension ref="B3:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
   </cols>
@@ -1122,14 +1127,15 @@
   <dimension ref="B3:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.5703125" customWidth="1"/>
-    <col min="5" max="5" width="25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
@@ -1244,12 +1250,14 @@
   <dimension ref="B3:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="B1" sqref="B1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="44.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="49.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1329,15 +1337,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BCEFDDC-10B1-4662-AC8B-41DA2BB9AB2A}">
   <dimension ref="B2:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.7109375" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1430,11 +1439,13 @@
   <dimension ref="B3:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.42578125" bestFit="1" customWidth="1"/>
   </cols>
@@ -1516,13 +1527,14 @@
   <dimension ref="B3:I13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="B1" sqref="B1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1593,13 +1605,14 @@
   <dimension ref="B3:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:E5"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.28515625" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1662,14 +1675,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F23CC946-F6E0-4EA9-AFCD-8670B9A50492}">
   <dimension ref="B3:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1727,7 +1741,7 @@
   <dimension ref="B2:H16"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="B1" sqref="B1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1735,7 +1749,7 @@
     <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="40.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="40.85546875" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="47.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1929,12 +1943,13 @@
   <dimension ref="B3:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A10:A15"/>
+      <selection activeCell="B1" sqref="B1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="19.85546875" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2032,13 +2047,17 @@
   <dimension ref="B2:J17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:C6"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="30" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="46.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2192,17 +2211,18 @@
   <dimension ref="B3:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H4" sqref="H4:H6"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="47.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="46" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="47.28515625" customWidth="1"/>
-    <col min="8" max="8" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="29.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
@@ -2333,13 +2353,16 @@
   <dimension ref="B2:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="47" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
@@ -2403,13 +2426,14 @@
   <dimension ref="B3:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="B1" sqref="B1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="42" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="43.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2494,18 +2518,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{945BD593-8DF0-43F2-BE97-815884B39FA6}">
   <dimension ref="B2:I5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="30.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="49.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="29.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="46" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="18.42578125" bestFit="1" customWidth="1"/>
   </cols>
@@ -2653,14 +2678,17 @@
   <dimension ref="B3:I17"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="B1" sqref="B1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.42578125" customWidth="1"/>
+    <col min="7" max="7" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="30.7109375" bestFit="1" customWidth="1"/>
   </cols>

</xml_diff>